<commit_message>
Excel apoyos corréctamente estructurado y funcionando, falta hacer cálculo días trabajados
</commit_message>
<xml_diff>
--- a/src/main/resources/MEDICIONES SAN LEONARDO URBA SUR 1 A 9 MARZO.xlsx
+++ b/src/main/resources/MEDICIONES SAN LEONARDO URBA SUR 1 A 9 MARZO.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\INES\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\INES\Desktop\ROBERTO\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6CA98867-382F-4E49-931B-81CF82F263EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12B57692-5EC8-4F0E-A3FE-7E459C123812}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C66C163A-FC94-45BE-AEE2-81A12E3FD87B}"/>
   </bookViews>
@@ -23,19 +23,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="33">
   <si>
     <t>DÍA</t>
   </si>
@@ -138,6 +131,15 @@
   <si>
     <t>1 H ESPERA</t>
   </si>
+  <si>
+    <t>PEPE</t>
+  </si>
+  <si>
+    <t>CAMBIO</t>
+  </si>
+  <si>
+    <t>HOLA</t>
+  </si>
 </sst>
 </file>
 
@@ -146,7 +148,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -193,6 +195,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -501,7 +511,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -592,6 +602,61 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -607,65 +672,11 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -984,10 +995,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:J37"/>
+  <dimension ref="B1:K37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="M22" sqref="M22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="R17" sqref="R17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1003,17 +1014,17 @@
   <sheetData>
     <row r="1" spans="2:10" ht="10.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:10" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="43" t="s">
+      <c r="B2" s="35" t="s">
         <v>26</v>
       </c>
-      <c r="C2" s="44"/>
-      <c r="D2" s="44"/>
-      <c r="E2" s="44"/>
-      <c r="F2" s="44"/>
-      <c r="G2" s="44"/>
-      <c r="H2" s="44"/>
-      <c r="I2" s="44"/>
-      <c r="J2" s="45"/>
+      <c r="C2" s="36"/>
+      <c r="D2" s="36"/>
+      <c r="E2" s="36"/>
+      <c r="F2" s="36"/>
+      <c r="G2" s="36"/>
+      <c r="H2" s="36"/>
+      <c r="I2" s="36"/>
+      <c r="J2" s="37"/>
     </row>
     <row r="3" spans="2:10" ht="8.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="2:10" ht="31.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1089,7 +1100,9 @@
       <c r="B7" s="26">
         <v>20</v>
       </c>
-      <c r="C7" s="27"/>
+      <c r="C7" s="27">
+        <v>20</v>
+      </c>
       <c r="D7" s="27"/>
       <c r="E7" s="27">
         <v>1</v>
@@ -1113,7 +1126,9 @@
       <c r="E8" s="27">
         <v>1</v>
       </c>
-      <c r="F8" s="27"/>
+      <c r="F8" s="27">
+        <v>3</v>
+      </c>
       <c r="G8" s="27"/>
       <c r="H8" s="28">
         <v>44621</v>
@@ -1128,12 +1143,16 @@
         <v>38</v>
       </c>
       <c r="C9" s="27"/>
-      <c r="D9" s="27"/>
+      <c r="D9" s="27">
+        <v>1</v>
+      </c>
       <c r="E9" s="27">
         <v>1</v>
       </c>
       <c r="F9" s="27"/>
-      <c r="G9" s="27"/>
+      <c r="G9" s="27">
+        <v>23</v>
+      </c>
       <c r="H9" s="28">
         <v>44629</v>
       </c>
@@ -1197,7 +1216,9 @@
       <c r="I12" s="29" t="s">
         <v>27</v>
       </c>
-      <c r="J12" s="29"/>
+      <c r="J12" s="29" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="13" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="26">
@@ -1216,7 +1237,9 @@
       <c r="I13" s="29" t="s">
         <v>27</v>
       </c>
-      <c r="J13" s="29"/>
+      <c r="J13" s="29" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="14" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="26">
@@ -1241,7 +1264,9 @@
       <c r="B15" s="26">
         <v>15497</v>
       </c>
-      <c r="C15" s="27"/>
+      <c r="C15" s="27">
+        <v>2000</v>
+      </c>
       <c r="D15" s="27"/>
       <c r="E15" s="27">
         <v>1</v>
@@ -1261,21 +1286,25 @@
         <v>15498</v>
       </c>
       <c r="C16" s="27"/>
-      <c r="D16" s="27"/>
+      <c r="D16" s="27">
+        <v>3100</v>
+      </c>
       <c r="E16" s="27">
         <v>1</v>
       </c>
       <c r="F16" s="27"/>
-      <c r="G16" s="27"/>
+      <c r="G16" s="27">
+        <v>1</v>
+      </c>
       <c r="H16" s="28">
         <v>44629</v>
       </c>
       <c r="I16" s="29" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="J16" s="29"/>
     </row>
-    <row r="17" spans="2:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:11" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B17" s="30">
         <v>25615</v>
       </c>
@@ -1290,21 +1319,22 @@
         <v>44623</v>
       </c>
       <c r="I17" s="33" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="J17" s="33"/>
-    </row>
-    <row r="18" spans="2:10" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K17" s="34"/>
+    </row>
+    <row r="18" spans="2:11" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B18" s="17" t="s">
         <v>5</v>
       </c>
       <c r="C18" s="15">
         <f>SUM(C5:C17)</f>
-        <v>0</v>
+        <v>2020</v>
       </c>
       <c r="D18" s="15">
         <f>SUM(D5:D17)</f>
-        <v>0</v>
+        <v>3101</v>
       </c>
       <c r="E18" s="15">
         <f>SUM(E5:E17)</f>
@@ -1312,51 +1342,51 @@
       </c>
       <c r="F18" s="15">
         <f>SUM(F5:F17)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G18" s="15">
         <f>SUM(G5:G17)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="2:10" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="19" spans="2:11" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B19" s="16" t="s">
         <v>6</v>
       </c>
       <c r="C19" s="13">
         <f>C18/1000</f>
-        <v>0</v>
+        <v>2.02</v>
       </c>
       <c r="D19" s="13">
         <f>D18/1000</f>
-        <v>0</v>
+        <v>3.101</v>
       </c>
       <c r="E19" s="13"/>
       <c r="F19" s="18">
         <f>F18</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G19" s="14">
         <f>G18</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="2:10" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="46"/>
-      <c r="C22" s="46"/>
-      <c r="D22" s="46"/>
-      <c r="E22" s="46"/>
-      <c r="F22" s="46"/>
-      <c r="G22" s="46"/>
-    </row>
-    <row r="23" spans="2:10" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="22" spans="2:11" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B22" s="38"/>
+      <c r="C22" s="38"/>
+      <c r="D22" s="38"/>
+      <c r="E22" s="38"/>
+      <c r="F22" s="38"/>
+      <c r="G22" s="38"/>
+    </row>
+    <row r="23" spans="2:11" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="7"/>
       <c r="C23" s="7"/>
       <c r="D23" s="8"/>
-      <c r="E23" s="52" t="s">
+      <c r="E23" s="44" t="s">
         <v>7</v>
       </c>
-      <c r="F23" s="53"/>
+      <c r="F23" s="45"/>
       <c r="G23" s="6" t="s">
         <v>8</v>
       </c>
@@ -1364,73 +1394,73 @@
         <v>10</v>
       </c>
     </row>
-    <row r="24" spans="2:10" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="49" t="s">
+    <row r="24" spans="2:11" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B24" s="41" t="s">
         <v>9</v>
       </c>
-      <c r="C24" s="50"/>
-      <c r="D24" s="51"/>
-      <c r="E24" s="54">
+      <c r="C24" s="42"/>
+      <c r="D24" s="43"/>
+      <c r="E24" s="46">
         <f>C19</f>
-        <v>0</v>
-      </c>
-      <c r="F24" s="55"/>
+        <v>2.02</v>
+      </c>
+      <c r="F24" s="47"/>
       <c r="G24" s="1">
         <v>3545.2</v>
       </c>
       <c r="H24" s="1">
         <f>E24*G24</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="2:10" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="49" t="s">
+        <v>7161.3040000000001</v>
+      </c>
+    </row>
+    <row r="25" spans="2:11" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B25" s="41" t="s">
         <v>16</v>
       </c>
-      <c r="C25" s="50"/>
-      <c r="D25" s="51"/>
-      <c r="E25" s="54">
+      <c r="C25" s="42"/>
+      <c r="D25" s="43"/>
+      <c r="E25" s="46">
         <f>D19</f>
-        <v>0</v>
-      </c>
-      <c r="F25" s="55"/>
+        <v>3.101</v>
+      </c>
+      <c r="F25" s="47"/>
       <c r="G25" s="1">
         <v>7090.4</v>
       </c>
       <c r="H25" s="1">
         <f>E25*G25</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>21987.330399999999</v>
+      </c>
+    </row>
+    <row r="26" spans="2:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" s="2" t="s">
         <v>11</v>
       </c>
       <c r="C26" s="2"/>
       <c r="D26" s="2"/>
-      <c r="E26" s="39">
+      <c r="E26" s="48">
         <f>F18</f>
-        <v>0</v>
-      </c>
-      <c r="F26" s="40"/>
+        <v>3</v>
+      </c>
+      <c r="F26" s="49"/>
       <c r="G26" s="1">
         <v>6.01</v>
       </c>
       <c r="H26" s="1">
         <f>E26*G26</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="2:10" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+        <v>18.03</v>
+      </c>
+    </row>
+    <row r="27" spans="2:11" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B27" s="2" t="s">
         <v>12</v>
       </c>
       <c r="C27" s="2"/>
       <c r="D27" s="2"/>
-      <c r="E27" s="39">
+      <c r="E27" s="48">
         <v>0</v>
       </c>
-      <c r="F27" s="40"/>
+      <c r="F27" s="49"/>
       <c r="G27" s="1">
         <v>10</v>
       </c>
@@ -1439,16 +1469,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="2:10" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="56" t="s">
+    <row r="28" spans="2:11" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B28" s="50" t="s">
         <v>24</v>
       </c>
-      <c r="C28" s="57"/>
-      <c r="D28" s="58"/>
-      <c r="E28" s="39">
+      <c r="C28" s="51"/>
+      <c r="D28" s="52"/>
+      <c r="E28" s="48">
         <v>0</v>
       </c>
-      <c r="F28" s="40"/>
+      <c r="F28" s="49"/>
       <c r="G28" s="3">
         <v>240.45</v>
       </c>
@@ -1457,16 +1487,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="2:10" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="35" t="s">
+    <row r="29" spans="2:11" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B29" s="54" t="s">
         <v>19</v>
       </c>
-      <c r="C29" s="36"/>
-      <c r="D29" s="37"/>
-      <c r="E29" s="39">
+      <c r="C29" s="55"/>
+      <c r="D29" s="56"/>
+      <c r="E29" s="48">
         <v>0</v>
       </c>
-      <c r="F29" s="40"/>
+      <c r="F29" s="49"/>
       <c r="G29" s="3">
         <v>50</v>
       </c>
@@ -1475,21 +1505,21 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="2:10" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="47" t="s">
+    <row r="30" spans="2:11" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B30" s="39" t="s">
         <v>22</v>
       </c>
-      <c r="C30" s="48"/>
-      <c r="D30" s="48"/>
-      <c r="E30" s="48"/>
-      <c r="F30" s="48"/>
-      <c r="G30" s="48"/>
+      <c r="C30" s="40"/>
+      <c r="D30" s="40"/>
+      <c r="E30" s="40"/>
+      <c r="F30" s="40"/>
+      <c r="G30" s="40"/>
       <c r="H30" s="4">
         <f>SUM(H24:H29)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="2:10" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>29166.664399999998</v>
+      </c>
+    </row>
+    <row r="31" spans="2:11" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B31" s="20" t="s">
         <v>23</v>
       </c>
@@ -1500,20 +1530,20 @@
       <c r="G31" s="21"/>
       <c r="H31" s="4">
         <f>H30*0.98</f>
-        <v>0</v>
+        <v>28583.331111999996</v>
       </c>
     </row>
     <row r="33" spans="2:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B33" s="34" t="s">
+      <c r="B33" s="53" t="s">
         <v>18</v>
       </c>
-      <c r="C33" s="34"/>
-      <c r="D33" s="34"/>
-      <c r="E33" s="38">
+      <c r="C33" s="53"/>
+      <c r="D33" s="53"/>
+      <c r="E33" s="57">
         <f>E18</f>
         <v>13</v>
       </c>
-      <c r="F33" s="38"/>
+      <c r="F33" s="57"/>
       <c r="G33" s="1">
         <v>250</v>
       </c>
@@ -1523,15 +1553,15 @@
       </c>
     </row>
     <row r="34" spans="2:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B34" s="34" t="s">
+      <c r="B34" s="53" t="s">
         <v>13</v>
       </c>
-      <c r="C34" s="34"/>
-      <c r="D34" s="34"/>
-      <c r="E34" s="38">
+      <c r="C34" s="53"/>
+      <c r="D34" s="53"/>
+      <c r="E34" s="57">
         <v>1</v>
       </c>
-      <c r="F34" s="38"/>
+      <c r="F34" s="57"/>
       <c r="G34" s="1">
         <v>90</v>
       </c>
@@ -1541,15 +1571,15 @@
       </c>
     </row>
     <row r="35" spans="2:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B35" s="34" t="s">
+      <c r="B35" s="53" t="s">
         <v>24</v>
       </c>
-      <c r="C35" s="34"/>
-      <c r="D35" s="34"/>
-      <c r="E35" s="38">
+      <c r="C35" s="53"/>
+      <c r="D35" s="53"/>
+      <c r="E35" s="57">
         <v>0</v>
       </c>
-      <c r="F35" s="38"/>
+      <c r="F35" s="57"/>
       <c r="G35" s="1">
         <v>240.45</v>
       </c>
@@ -1560,13 +1590,13 @@
     </row>
     <row r="36" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="37" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F37" s="41" t="s">
+      <c r="F37" s="58" t="s">
         <v>21</v>
       </c>
-      <c r="G37" s="42"/>
+      <c r="G37" s="59"/>
       <c r="H37" s="4">
         <f>H31+H33+H34+H35</f>
-        <v>3340</v>
+        <v>31923.331111999996</v>
       </c>
     </row>
   </sheetData>
@@ -1574,6 +1604,15 @@
     <sortCondition ref="B5:B17"/>
   </sortState>
   <mergeCells count="21">
+    <mergeCell ref="B33:D33"/>
+    <mergeCell ref="B29:D29"/>
+    <mergeCell ref="E33:F33"/>
+    <mergeCell ref="E29:F29"/>
+    <mergeCell ref="F37:G37"/>
+    <mergeCell ref="B34:D34"/>
+    <mergeCell ref="E34:F34"/>
+    <mergeCell ref="B35:D35"/>
+    <mergeCell ref="E35:F35"/>
     <mergeCell ref="B2:J2"/>
     <mergeCell ref="B22:G22"/>
     <mergeCell ref="B30:G30"/>
@@ -1586,15 +1625,6 @@
     <mergeCell ref="E27:F27"/>
     <mergeCell ref="B28:D28"/>
     <mergeCell ref="E28:F28"/>
-    <mergeCell ref="B33:D33"/>
-    <mergeCell ref="B29:D29"/>
-    <mergeCell ref="E33:F33"/>
-    <mergeCell ref="E29:F29"/>
-    <mergeCell ref="F37:G37"/>
-    <mergeCell ref="B34:D34"/>
-    <mergeCell ref="E34:F34"/>
-    <mergeCell ref="B35:D35"/>
-    <mergeCell ref="E35:F35"/>
   </mergeCells>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.55118110236220474" bottom="0.55118110236220474" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="72" fitToHeight="0" orientation="portrait" r:id="rId1"/>

</xml_diff>